<commit_message>
Add Intel KNL results
</commit_message>
<xml_diff>
--- a/results/train/DeepBench_IA_KNL7250.xlsx
+++ b/results/train/DeepBench_IA_KNL7250.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="32800" windowHeight="20080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Results - FP32" sheetId="3" r:id="rId1"/>
@@ -814,7 +814,7 @@
   <dimension ref="A1:AE369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3216,11 +3216,12 @@
         <v>8</v>
       </c>
       <c r="I98" s="2">
-        <v>147.66284045419013</v>
+        <f>144847.5/1000</f>
+        <v>144.8475</v>
       </c>
       <c r="J98" s="2">
         <f t="shared" si="5"/>
-        <v>4.0902624799999998</v>
+        <v>4.169763206130586</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -3342,11 +3343,12 @@
         <v>8</v>
       </c>
       <c r="I103" s="2">
-        <v>281.19163058905355</v>
+        <f>285128.3/1000</f>
+        <v>285.12829999999997</v>
       </c>
       <c r="J103" s="2">
         <f t="shared" si="5"/>
-        <v>4.2958588399999993</v>
+        <v>4.2365473788466463</v>
       </c>
     </row>
     <row r="104" spans="1:10">
@@ -3468,11 +3470,12 @@
         <v>8</v>
       </c>
       <c r="I108" s="2">
-        <v>151.0735982028003</v>
+        <f>144892.5/1000</f>
+        <v>144.89250000000001</v>
       </c>
       <c r="J108" s="2">
         <f t="shared" si="5"/>
-        <v>3.99791746</v>
+        <v>4.1684681815828979</v>
       </c>
     </row>
     <row r="109" spans="1:10">
@@ -3594,11 +3597,12 @@
         <v>8</v>
       </c>
       <c r="I113" s="2">
-        <v>295.3189056155382</v>
+        <f>286129.4/1000</f>
+        <v>286.12940000000003</v>
       </c>
       <c r="J113" s="2">
         <f t="shared" si="5"/>
-        <v>4.0903563199999997</v>
+        <v>4.2217246882005135</v>
       </c>
     </row>
     <row r="114" spans="1:10">
@@ -3698,11 +3702,11 @@
       </c>
       <c r="H117" s="3"/>
       <c r="I117" s="2">
-        <v>0.2440202949586612</v>
+        <v>0.27300000000000002</v>
       </c>
       <c r="J117" s="2">
         <f t="shared" si="5"/>
-        <v>1.6500807199999998</v>
+        <v>1.4749200879120878</v>
       </c>
     </row>
     <row r="118" spans="1:10">
@@ -3776,11 +3780,11 @@
       </c>
       <c r="H120" s="3"/>
       <c r="I120" s="2">
-        <v>0.31639999887003706</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="J120" s="2">
         <f t="shared" si="5"/>
-        <v>2.5452160899999994</v>
+        <v>2.3546969824561401</v>
       </c>
     </row>
     <row r="121" spans="1:10">
@@ -3854,11 +3858,11 @@
       </c>
       <c r="H123" s="3"/>
       <c r="I123" s="2">
-        <v>0.24397619361356512</v>
+        <v>0.26200000000000001</v>
       </c>
       <c r="J123" s="2">
         <f t="shared" si="5"/>
-        <v>1.6503789899999997</v>
+        <v>1.5368442137404577</v>
       </c>
     </row>
     <row r="124" spans="1:10">
@@ -3932,11 +3936,11 @@
       </c>
       <c r="H126" s="3"/>
       <c r="I126" s="2">
-        <v>0.31805180720836901</v>
+        <v>0.34899999999999998</v>
       </c>
       <c r="J126" s="2">
         <f t="shared" si="5"/>
-        <v>2.5319974599999999</v>
+        <v>2.3074681031518627</v>
       </c>
     </row>
     <row r="127" spans="1:10">

</xml_diff>